<commit_message>
Renamed Trade type values
</commit_message>
<xml_diff>
--- a/CryptoTradeStats/Sample Logbook/SampleLogbook.xlsx
+++ b/CryptoTradeStats/Sample Logbook/SampleLogbook.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yash.Gupta\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yash.Gupta\source\repos\CryptoTradeStats\CryptoTradeStats\Sample Logbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4692B3B4-2FCB-4D67-BAFD-84178ABC4E6B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9874C53C-BB7D-4774-BF1F-C0C4F49D0272}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1327747F-1C0B-489C-8E3C-87F7E959DC26}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{1327747F-1C0B-489C-8E3C-87F7E959DC26}"/>
   </bookViews>
   <sheets>
     <sheet name="USDT" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="19">
   <si>
     <t>Date-Time</t>
   </si>
@@ -76,34 +76,22 @@
     <t>Total Sell Price (BTC)</t>
   </si>
   <si>
-    <t>Deposit (INR)</t>
-  </si>
-  <si>
     <t>ABC</t>
   </si>
   <si>
     <t>XYZ</t>
   </si>
   <si>
-    <t>Withdraw (BTC)</t>
-  </si>
-  <si>
     <t>DEF</t>
   </si>
   <si>
-    <t>Reinvest (BTC)</t>
-  </si>
-  <si>
-    <t>IJK</t>
-  </si>
-  <si>
-    <t>Withdraw (INR)</t>
-  </si>
-  <si>
-    <t>Reinvest (USDT)</t>
-  </si>
-  <si>
-    <t>Withdraw (USDT)</t>
+    <t>Buy</t>
+  </si>
+  <si>
+    <t>Reinvest</t>
+  </si>
+  <si>
+    <t>Sell</t>
   </si>
 </sst>
 </file>
@@ -517,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{113E35F4-1294-420B-A0A4-18F3E49CC8C0}">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -581,7 +569,7 @@
         <v>44360</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" s="6">
         <v>0</v>
@@ -603,7 +591,7 @@
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
       <c r="L2" s="6" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -611,7 +599,7 @@
         <v>44360</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C3" s="6">
         <v>0</v>
@@ -633,7 +621,7 @@
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
       <c r="L3" s="6" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -641,7 +629,7 @@
         <v>44360</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C4" s="6">
         <v>0</v>
@@ -663,37 +651,7 @@
         <v>0</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="7">
-        <v>44360</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="6">
-        <v>0</v>
-      </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6">
-        <v>0</v>
-      </c>
-      <c r="I5" s="6">
-        <v>0</v>
-      </c>
-      <c r="J5" s="6">
-        <v>0</v>
-      </c>
-      <c r="K5" s="6">
-        <v>0</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -703,10 +661,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{007DC722-8B6F-462F-AF79-533A35929D35}">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -767,7 +725,7 @@
         <v>44360</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" s="6">
         <v>0</v>
@@ -789,7 +747,7 @@
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
       <c r="L2" s="6" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -797,7 +755,7 @@
         <v>44360</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C3" s="6">
         <v>0</v>
@@ -819,7 +777,7 @@
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
       <c r="L3" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -827,7 +785,7 @@
         <v>44360</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C4" s="6">
         <v>0</v>
@@ -849,33 +807,7 @@
         <v>0</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="7">
-        <v>44360</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="6">
-        <v>0</v>
-      </c>
-      <c r="H5" s="6">
-        <v>0</v>
-      </c>
-      <c r="I5" s="6">
-        <v>0</v>
-      </c>
-      <c r="J5" s="6">
-        <v>0</v>
-      </c>
-      <c r="K5" s="6">
-        <v>0</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>